<commit_message>
Did entry counts through section 66 in AAA 19
 On branch master

 Changes to be committed:
	modified:   Books20/Data/AAA/AAA_counts.xlsx
</commit_message>
<xml_diff>
--- a/Books20/Data/AAA/AAA_counts.xlsx
+++ b/Books20/Data/AAA/AAA_counts.xlsx
@@ -58349,8 +58349,8 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -58393,7 +58393,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>1290</v>
+        <v>2096</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -58951,7 +58951,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="n">
         <f aca="false">SUM(F36:F42)</f>
-        <v>0</v>
+        <v>232</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -58968,7 +58968,9 @@
         <v>35</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="n">
+        <v>42</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
@@ -58984,7 +58986,9 @@
         <v>172</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="11" t="n">
+        <v>61</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
@@ -59000,7 +59004,9 @@
         <v>37</v>
       </c>
       <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="11" t="n">
+        <v>7</v>
+      </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
@@ -59016,7 +59022,9 @@
         <v>38</v>
       </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11" t="n">
+        <v>38</v>
+      </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
@@ -59032,7 +59040,9 @@
         <v>39</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11" t="n">
+        <v>30</v>
+      </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
@@ -59048,7 +59058,9 @@
         <v>173</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
     </row>
@@ -59064,7 +59076,9 @@
         <v>41</v>
       </c>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="n">
+        <v>29</v>
+      </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
@@ -59080,7 +59094,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="n">
         <f aca="false">SUM(F44:F48)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -59097,7 +59111,9 @@
         <v>174</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
@@ -59113,7 +59129,9 @@
         <v>44</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
@@ -59129,7 +59147,9 @@
         <v>45</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="n">
+        <v>12</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
@@ -59145,7 +59165,9 @@
         <v>46</v>
       </c>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="n">
+        <v>23</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
@@ -59161,7 +59183,9 @@
         <v>47</v>
       </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="n">
+        <v>13</v>
+      </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
@@ -59177,7 +59201,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10" t="n">
         <f aca="false">SUM(F50:F55)</f>
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -59194,7 +59218,9 @@
         <v>49</v>
       </c>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="n">
+        <v>60</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
     </row>
@@ -59210,7 +59236,9 @@
         <v>163</v>
       </c>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="n">
+        <v>76</v>
+      </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
@@ -59226,7 +59254,9 @@
         <v>148</v>
       </c>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="n">
+        <v>37</v>
+      </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
     </row>
@@ -59242,7 +59272,9 @@
         <v>175</v>
       </c>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="F53" s="11" t="n">
+        <v>54</v>
+      </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
     </row>
@@ -59258,7 +59290,9 @@
         <v>191</v>
       </c>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="F54" s="11" t="n">
+        <v>80</v>
+      </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
@@ -59274,7 +59308,9 @@
         <v>192</v>
       </c>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11" t="n">
+        <v>157</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
     </row>

</xml_diff>

<commit_message>
Finished entry counts for AAA 20
 On branch master

 Changes to be committed:
	modified:   Data/AAA/AAA_counts.xlsx
	modified:   Data/Ajb/ajb.ods
</commit_message>
<xml_diff>
--- a/Books20/Data/AAA/AAA_counts.xlsx
+++ b/Books20/Data/AAA/AAA_counts.xlsx
@@ -1231,13 +1231,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3653,7 +3653,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3668,17 +3668,17 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>1413</v>
+        <v>7579</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -4271,7 +4271,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="n">
         <f aca="false">SUM(F36:F42)</f>
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -4288,7 +4288,9 @@
         <v>203</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="n">
+        <v>55</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
@@ -4304,7 +4306,9 @@
         <v>172</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="11" t="n">
+        <v>80</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
@@ -4320,7 +4324,9 @@
         <v>37</v>
       </c>
       <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
@@ -4336,7 +4342,9 @@
         <v>38</v>
       </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11" t="n">
+        <v>43</v>
+      </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
@@ -4352,7 +4360,9 @@
         <v>39</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
@@ -4368,7 +4378,9 @@
         <v>173</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11" t="n">
+        <v>76</v>
+      </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
     </row>
@@ -4384,7 +4396,9 @@
         <v>41</v>
       </c>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
@@ -4400,7 +4414,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="n">
         <f aca="false">SUM(F44:F48)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -4417,7 +4431,9 @@
         <v>174</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
@@ -4433,7 +4449,9 @@
         <v>44</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
@@ -4449,7 +4467,9 @@
         <v>45</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
@@ -4465,7 +4485,9 @@
         <v>46</v>
       </c>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
@@ -4481,7 +4503,9 @@
         <v>47</v>
       </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
@@ -4497,7 +4521,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10" t="n">
         <f aca="false">SUM(F50:F55)</f>
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4514,7 +4538,9 @@
         <v>49</v>
       </c>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="n">
+        <v>53</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
     </row>
@@ -4530,7 +4556,9 @@
         <v>163</v>
       </c>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="n">
+        <v>84</v>
+      </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
@@ -4546,7 +4574,9 @@
         <v>148</v>
       </c>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="n">
+        <v>56</v>
+      </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
     </row>
@@ -4562,7 +4592,9 @@
         <v>175</v>
       </c>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="F53" s="11" t="n">
+        <v>61</v>
+      </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
     </row>
@@ -4578,7 +4610,9 @@
         <v>191</v>
       </c>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="F54" s="11" t="n">
+        <v>85</v>
+      </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
@@ -4594,7 +4628,9 @@
         <v>192</v>
       </c>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11" t="n">
+        <v>380</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
     </row>
@@ -4610,7 +4646,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10" t="n">
         <f aca="false">SUM(F57:F65,F68)</f>
-        <v>0</v>
+        <v>607</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -4627,7 +4663,9 @@
         <v>56</v>
       </c>
       <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+      <c r="F57" s="11" t="n">
+        <v>59</v>
+      </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
     </row>
@@ -4643,7 +4681,9 @@
         <v>57</v>
       </c>
       <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="F58" s="11" t="n">
+        <v>61</v>
+      </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
     </row>
@@ -4659,7 +4699,9 @@
         <v>58</v>
       </c>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="F59" s="11" t="n">
+        <v>123</v>
+      </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
     </row>
@@ -4675,7 +4717,9 @@
         <v>142</v>
       </c>
       <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="F60" s="11" t="n">
+        <v>122</v>
+      </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
     </row>
@@ -4691,7 +4735,9 @@
         <v>60</v>
       </c>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="F61" s="11" t="n">
+        <v>26</v>
+      </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
     </row>
@@ -4707,7 +4753,9 @@
         <v>177</v>
       </c>
       <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="F62" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
     </row>
@@ -4723,7 +4771,9 @@
         <v>62</v>
       </c>
       <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="F63" s="11" t="n">
+        <v>57</v>
+      </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
     </row>
@@ -4739,7 +4789,9 @@
         <v>63</v>
       </c>
       <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
+      <c r="F64" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
     </row>
@@ -4757,7 +4809,7 @@
       <c r="E65" s="11"/>
       <c r="F65" s="18" t="n">
         <f aca="false">SUM(F66:F67)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -4772,7 +4824,9 @@
         <v>64</v>
       </c>
       <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
+      <c r="F66" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
     </row>
@@ -4786,7 +4840,9 @@
         <v>149</v>
       </c>
       <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="16" t="n">
+        <v>21</v>
+      </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
     </row>
@@ -4802,7 +4858,9 @@
         <v>178</v>
       </c>
       <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="F68" s="11" t="n">
+        <v>96</v>
+      </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
     </row>
@@ -4818,7 +4876,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="10" t="n">
         <f aca="false">SUM(F70:F73,F77)</f>
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
@@ -4835,7 +4893,9 @@
         <v>204</v>
       </c>
       <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="F70" s="11" t="n">
+        <v>72</v>
+      </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
     </row>
@@ -4851,7 +4911,9 @@
         <v>205</v>
       </c>
       <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="F71" s="11" t="n">
+        <v>145</v>
+      </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
     </row>
@@ -4867,7 +4929,9 @@
         <v>71</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+      <c r="F72" s="11" t="n">
+        <v>144</v>
+      </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
     </row>
@@ -4885,7 +4949,7 @@
       <c r="E73" s="11"/>
       <c r="F73" s="11" t="n">
         <f aca="false">SUM(F74:F76)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -4900,7 +4964,9 @@
         <v>73</v>
       </c>
       <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="16" t="n">
+        <v>40</v>
+      </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
     </row>
@@ -4914,7 +4980,9 @@
         <v>74</v>
       </c>
       <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
+      <c r="F75" s="16" t="n">
+        <v>123</v>
+      </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
     </row>
@@ -4928,7 +4996,9 @@
         <v>75</v>
       </c>
       <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
+      <c r="F76" s="16" t="n">
+        <v>5</v>
+      </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
@@ -4944,7 +5014,9 @@
         <v>76</v>
       </c>
       <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+      <c r="F77" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
     </row>
@@ -4960,7 +5032,7 @@
       <c r="E78" s="10"/>
       <c r="F78" s="10" t="n">
         <f aca="false">SUM(F79:F82,F86:F88,F92,F95,F98:F100,F103:F106)</f>
-        <v>0</v>
+        <v>1521</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
@@ -4977,7 +5049,9 @@
         <v>179</v>
       </c>
       <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="F79" s="11" t="n">
+        <v>84</v>
+      </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
     </row>
@@ -4993,7 +5067,9 @@
         <v>79</v>
       </c>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="F80" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
     </row>
@@ -5009,7 +5085,9 @@
         <v>80</v>
       </c>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
+      <c r="F81" s="11" t="n">
+        <v>71</v>
+      </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
     </row>
@@ -5027,7 +5105,7 @@
       <c r="E82" s="11"/>
       <c r="F82" s="11" t="n">
         <f aca="false">SUM(F83:F85)</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -5042,7 +5120,9 @@
         <v>150</v>
       </c>
       <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
+      <c r="F83" s="16" t="n">
+        <v>17</v>
+      </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
     </row>
@@ -5056,7 +5136,9 @@
         <v>151</v>
       </c>
       <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
+      <c r="F84" s="16" t="n">
+        <v>101</v>
+      </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
     </row>
@@ -5070,7 +5152,9 @@
         <v>152</v>
       </c>
       <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="F85" s="16" t="n">
+        <v>113</v>
+      </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
     </row>
@@ -5086,7 +5170,9 @@
         <v>82</v>
       </c>
       <c r="E86" s="11"/>
-      <c r="F86" s="17"/>
+      <c r="F86" s="17" t="n">
+        <v>3</v>
+      </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
     </row>
@@ -5102,7 +5188,9 @@
         <v>83</v>
       </c>
       <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="F87" s="11" t="n">
+        <v>28</v>
+      </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
     </row>
@@ -5120,7 +5208,7 @@
       <c r="E88" s="11"/>
       <c r="F88" s="11" t="n">
         <f aca="false">SUM(F89:F90)</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -5135,7 +5223,9 @@
         <v>84</v>
       </c>
       <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
+      <c r="F89" s="16" t="n">
+        <v>219</v>
+      </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
     </row>
@@ -5149,7 +5239,9 @@
         <v>153</v>
       </c>
       <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
+      <c r="F90" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
     </row>
@@ -5165,7 +5257,9 @@
         <v>85</v>
       </c>
       <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="F91" s="11" t="n">
+        <v>107</v>
+      </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
     </row>
@@ -5183,7 +5277,7 @@
       <c r="E92" s="11"/>
       <c r="F92" s="11" t="n">
         <f aca="false">SUM(F93:F94)</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -5198,7 +5292,9 @@
         <v>86</v>
       </c>
       <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
+      <c r="F93" s="16" t="n">
+        <v>86</v>
+      </c>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
     </row>
@@ -5212,7 +5308,9 @@
         <v>154</v>
       </c>
       <c r="E94" s="16"/>
-      <c r="F94" s="16"/>
+      <c r="F94" s="16" t="n">
+        <v>18</v>
+      </c>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
     </row>
@@ -5230,7 +5328,7 @@
       <c r="E95" s="11"/>
       <c r="F95" s="11" t="n">
         <f aca="false">SUM(F96:F97)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -5245,7 +5343,9 @@
         <v>87</v>
       </c>
       <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
+      <c r="F96" s="16" t="n">
+        <v>35</v>
+      </c>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
     </row>
@@ -5259,7 +5359,9 @@
         <v>155</v>
       </c>
       <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
+      <c r="F97" s="16" t="n">
+        <v>14</v>
+      </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
     </row>
@@ -5275,7 +5377,9 @@
         <v>88</v>
       </c>
       <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="F98" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
     </row>
@@ -5291,7 +5395,9 @@
         <v>89</v>
       </c>
       <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="F99" s="11" t="n">
+        <v>56</v>
+      </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
     </row>
@@ -5309,7 +5415,7 @@
       <c r="E100" s="11"/>
       <c r="F100" s="11" t="n">
         <f aca="false">SUM(F101:F102)</f>
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
@@ -5324,7 +5430,9 @@
         <v>65</v>
       </c>
       <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
+      <c r="F101" s="16" t="n">
+        <v>8</v>
+      </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
     </row>
@@ -5338,7 +5446,9 @@
         <v>156</v>
       </c>
       <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
+      <c r="F102" s="16" t="n">
+        <v>105</v>
+      </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
     </row>
@@ -5354,7 +5464,9 @@
         <v>92</v>
       </c>
       <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="F103" s="11" t="n">
+        <v>59</v>
+      </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
     </row>
@@ -5370,7 +5482,9 @@
         <v>93</v>
       </c>
       <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
+      <c r="F104" s="11" t="n">
+        <v>288</v>
+      </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
     </row>
@@ -5386,7 +5500,9 @@
         <v>94</v>
       </c>
       <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
+      <c r="F105" s="11" t="n">
+        <v>51</v>
+      </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
     </row>
@@ -5402,7 +5518,9 @@
         <v>95</v>
       </c>
       <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
+      <c r="F106" s="11" t="n">
+        <v>63</v>
+      </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
     </row>
@@ -5418,7 +5536,7 @@
       <c r="E107" s="10"/>
       <c r="F107" s="10" t="n">
         <f aca="false">SUM(F108:F111,F114:F123,F126,F129)</f>
-        <v>0</v>
+        <v>797</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
@@ -5435,7 +5553,9 @@
         <v>206</v>
       </c>
       <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
+      <c r="F108" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
     </row>
@@ -5451,7 +5571,9 @@
         <v>98</v>
       </c>
       <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
+      <c r="F109" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
     </row>
@@ -5467,7 +5589,9 @@
         <v>99</v>
       </c>
       <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
+      <c r="F110" s="11" t="n">
+        <v>46</v>
+      </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
@@ -5485,7 +5609,7 @@
       <c r="E111" s="11"/>
       <c r="F111" s="11" t="n">
         <f aca="false">SUM(F112:F113)</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
@@ -5500,7 +5624,9 @@
         <v>100</v>
       </c>
       <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
+      <c r="F112" s="11" t="n">
+        <v>71</v>
+      </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
     </row>
@@ -5514,7 +5640,9 @@
         <v>180</v>
       </c>
       <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="F113" s="11" t="n">
+        <v>63</v>
+      </c>
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
     </row>
@@ -5530,7 +5658,9 @@
         <v>144</v>
       </c>
       <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="F114" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
@@ -5546,7 +5676,9 @@
         <v>102</v>
       </c>
       <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
+      <c r="F115" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
@@ -5562,7 +5694,9 @@
         <v>185</v>
       </c>
       <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
+      <c r="F116" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
@@ -5578,7 +5712,9 @@
         <v>165</v>
       </c>
       <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
+      <c r="F117" s="11" t="n">
+        <v>41</v>
+      </c>
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
@@ -5594,7 +5730,9 @@
         <v>105</v>
       </c>
       <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+      <c r="F118" s="11" t="n">
+        <v>17</v>
+      </c>
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
@@ -5610,7 +5748,9 @@
         <v>207</v>
       </c>
       <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
+      <c r="F119" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
@@ -5626,7 +5766,9 @@
         <v>107</v>
       </c>
       <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
+      <c r="F120" s="11" t="n">
+        <v>102</v>
+      </c>
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
@@ -5642,7 +5784,9 @@
         <v>166</v>
       </c>
       <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
+      <c r="F121" s="11" t="n">
+        <v>172</v>
+      </c>
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
@@ -5658,7 +5802,9 @@
         <v>109</v>
       </c>
       <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
+      <c r="F122" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
@@ -5676,7 +5822,7 @@
       <c r="E123" s="11"/>
       <c r="F123" s="11" t="n">
         <f aca="false">SUM(F124:F125)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
@@ -5691,7 +5837,9 @@
         <v>65</v>
       </c>
       <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
+      <c r="F124" s="11" t="n">
+        <v>9</v>
+      </c>
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
@@ -5705,7 +5853,9 @@
         <v>111</v>
       </c>
       <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
+      <c r="F125" s="11" t="n">
+        <v>36</v>
+      </c>
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
@@ -5723,7 +5873,7 @@
       <c r="E126" s="11"/>
       <c r="F126" s="11" t="n">
         <f aca="false">SUM(F127:F128)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
@@ -5738,7 +5888,9 @@
         <v>65</v>
       </c>
       <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
+      <c r="F127" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
@@ -5752,7 +5904,9 @@
         <v>114</v>
       </c>
       <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
+      <c r="F128" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
@@ -5768,7 +5922,9 @@
         <v>115</v>
       </c>
       <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
+      <c r="F129" s="11" t="n">
+        <v>22</v>
+      </c>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
     </row>
@@ -5784,7 +5940,7 @@
       <c r="E130" s="10"/>
       <c r="F130" s="10" t="n">
         <f aca="false">SUM(F131:F135)</f>
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
@@ -5801,7 +5957,9 @@
         <v>196</v>
       </c>
       <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
+      <c r="F131" s="11" t="n">
+        <v>222</v>
+      </c>
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
     </row>
@@ -5817,7 +5975,9 @@
         <v>158</v>
       </c>
       <c r="E132" s="17"/>
-      <c r="F132" s="17"/>
+      <c r="F132" s="17" t="n">
+        <v>39</v>
+      </c>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
@@ -5833,7 +5993,9 @@
         <v>159</v>
       </c>
       <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
+      <c r="F133" s="17" t="n">
+        <v>18</v>
+      </c>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
@@ -5849,7 +6011,9 @@
         <v>118</v>
       </c>
       <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
+      <c r="F134" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
@@ -5865,7 +6029,9 @@
         <v>119</v>
       </c>
       <c r="E135" s="11"/>
-      <c r="F135" s="11"/>
+      <c r="F135" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
     </row>
@@ -5881,7 +6047,7 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10" t="n">
         <f aca="false">SUM(F137,F140,F143)</f>
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="G136" s="11"/>
       <c r="H136" s="11"/>
@@ -5900,7 +6066,7 @@
       <c r="E137" s="11"/>
       <c r="F137" s="11" t="n">
         <f aca="false">SUM(F138:F139)</f>
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="G137" s="11"/>
       <c r="H137" s="11"/>
@@ -5915,7 +6081,9 @@
         <v>123</v>
       </c>
       <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
+      <c r="F138" s="16" t="n">
+        <v>166</v>
+      </c>
       <c r="G138" s="11"/>
       <c r="H138" s="11"/>
     </row>
@@ -5929,7 +6097,9 @@
         <v>124</v>
       </c>
       <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
+      <c r="F139" s="16" t="n">
+        <v>52</v>
+      </c>
       <c r="G139" s="11"/>
       <c r="H139" s="11"/>
     </row>
@@ -5947,7 +6117,7 @@
       <c r="E140" s="11"/>
       <c r="F140" s="11" t="n">
         <f aca="false">SUM(F141:F142)</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
@@ -5962,7 +6132,9 @@
         <v>197</v>
       </c>
       <c r="E141" s="16"/>
-      <c r="F141" s="16"/>
+      <c r="F141" s="16" t="n">
+        <v>138</v>
+      </c>
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
     </row>
@@ -5976,7 +6148,9 @@
         <v>198</v>
       </c>
       <c r="E142" s="16"/>
-      <c r="F142" s="16"/>
+      <c r="F142" s="16" t="n">
+        <v>14</v>
+      </c>
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
     </row>
@@ -5992,7 +6166,9 @@
         <v>63</v>
       </c>
       <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
+      <c r="F143" s="11" t="n">
+        <v>78</v>
+      </c>
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
     </row>
@@ -6008,7 +6184,7 @@
       <c r="E144" s="10"/>
       <c r="F144" s="10" t="n">
         <f aca="false">SUM(F145:F152,F155:F158)</f>
-        <v>0</v>
+        <v>638</v>
       </c>
       <c r="G144" s="11"/>
       <c r="H144" s="11"/>
@@ -6025,7 +6201,9 @@
         <v>127</v>
       </c>
       <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
+      <c r="F145" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
     </row>
@@ -6041,7 +6219,9 @@
         <v>128</v>
       </c>
       <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
+      <c r="F146" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G146" s="11"/>
       <c r="H146" s="11"/>
     </row>
@@ -6057,7 +6237,9 @@
         <v>129</v>
       </c>
       <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
+      <c r="F147" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G147" s="11"/>
       <c r="H147" s="11"/>
     </row>
@@ -6073,7 +6255,9 @@
         <v>130</v>
       </c>
       <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="F148" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="G148" s="11"/>
       <c r="H148" s="11"/>
     </row>
@@ -6089,7 +6273,9 @@
         <v>131</v>
       </c>
       <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
+      <c r="F149" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="G149" s="11"/>
       <c r="H149" s="11"/>
     </row>
@@ -6105,7 +6291,9 @@
         <v>199</v>
       </c>
       <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
+      <c r="F150" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G150" s="11"/>
       <c r="H150" s="11"/>
     </row>
@@ -6121,7 +6309,9 @@
         <v>200</v>
       </c>
       <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="F151" s="11" t="n">
+        <v>17</v>
+      </c>
       <c r="G151" s="11"/>
       <c r="H151" s="11"/>
     </row>
@@ -6139,7 +6329,7 @@
       <c r="E152" s="11"/>
       <c r="F152" s="11" t="n">
         <f aca="false">SUM(F153:F154)</f>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G152" s="11"/>
       <c r="H152" s="11"/>
@@ -6154,7 +6344,9 @@
         <v>134</v>
       </c>
       <c r="E153" s="16"/>
-      <c r="F153" s="16"/>
+      <c r="F153" s="16" t="n">
+        <v>123</v>
+      </c>
       <c r="G153" s="11"/>
       <c r="H153" s="11"/>
     </row>
@@ -6168,7 +6360,9 @@
         <v>160</v>
       </c>
       <c r="E154" s="16"/>
-      <c r="F154" s="16"/>
+      <c r="F154" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="G154" s="11"/>
       <c r="H154" s="11"/>
     </row>
@@ -6184,7 +6378,9 @@
         <v>135</v>
       </c>
       <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
+      <c r="F155" s="11" t="n">
+        <v>14</v>
+      </c>
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
     </row>
@@ -6200,7 +6396,9 @@
         <v>136</v>
       </c>
       <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
+      <c r="F156" s="11" t="n">
+        <v>64</v>
+      </c>
       <c r="G156" s="11"/>
       <c r="H156" s="11"/>
     </row>
@@ -6216,7 +6414,9 @@
         <v>137</v>
       </c>
       <c r="E157" s="11"/>
-      <c r="F157" s="11"/>
+      <c r="F157" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G157" s="11"/>
       <c r="H157" s="11"/>
     </row>
@@ -6232,14 +6432,16 @@
         <v>138</v>
       </c>
       <c r="E158" s="11"/>
-      <c r="F158" s="11"/>
+      <c r="F158" s="11" t="n">
+        <v>130</v>
+      </c>
       <c r="G158" s="11"/>
       <c r="H158" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6258,13 +6460,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8779,7 +8981,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8798,10 +9000,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10127,7 +10329,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10146,10 +10348,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11478,7 +11680,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -11497,10 +11699,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12814,7 +13016,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12833,10 +13035,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14150,7 +14352,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14169,10 +14371,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15486,7 +15688,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15505,10 +15707,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16822,7 +17024,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -16841,10 +17043,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18158,7 +18360,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -18177,10 +18379,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19494,7 +19696,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -19513,13 +19715,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21820,7 +22022,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -21839,10 +22041,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23156,7 +23358,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -23175,10 +23377,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24492,7 +24694,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -24511,10 +24713,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25828,7 +26030,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -25847,10 +26049,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27164,7 +27366,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27183,10 +27385,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28500,7 +28702,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -28519,10 +28721,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29836,7 +30038,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29855,10 +30057,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31172,7 +31374,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -31191,10 +31393,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32508,7 +32710,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -32527,10 +32729,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33839,7 +34041,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -33858,10 +34060,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35170,7 +35372,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -35189,13 +35391,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37841,7 +38043,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -37860,10 +38062,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39172,7 +39374,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -39191,10 +39393,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40503,7 +40705,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -40522,10 +40724,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41834,7 +42036,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -41853,10 +42055,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43173,7 +43375,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -43192,10 +43394,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44504,7 +44706,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -44523,10 +44725,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45835,7 +46037,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -45854,10 +46056,10 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47166,7 +47368,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -47185,13 +47387,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49837,7 +50039,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -49856,13 +50058,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52592,7 +52794,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -52611,13 +52813,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55373,7 +55575,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -55392,13 +55594,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58159,7 +58361,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -58178,13 +58380,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60945,7 +61147,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -60964,13 +61166,13 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63732,7 +63934,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Merged conflicts with github and origin
I had made changed to this file on my Mac while in Cloudcroft,
then made changes on Biblion in Fort Davis prior to merging
these two repositories.  Had to add about 50% of AAA20 counts
by hand.

 On branch master

 Changes to be committed:
	modified:   Books20/Data/AAA/AAA_counts.xlsx
</commit_message>
<xml_diff>
--- a/Books20/Data/AAA/AAA_counts.xlsx
+++ b/Books20/Data/AAA/AAA_counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="AAA v9 1973.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -3681,8 +3681,8 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F159" activeCellId="0" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>1413</v>
+        <v>7579</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -4284,7 +4284,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="n">
         <f aca="false">SUM(F36:F42)</f>
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -4301,7 +4301,9 @@
         <v>203</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="n">
+        <v>55</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
@@ -4317,7 +4319,9 @@
         <v>172</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="11" t="n">
+        <v>80</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
@@ -4333,7 +4337,9 @@
         <v>37</v>
       </c>
       <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
@@ -4349,7 +4355,9 @@
         <v>38</v>
       </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11" t="n">
+        <v>43</v>
+      </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
@@ -4365,7 +4373,9 @@
         <v>39</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
@@ -4381,7 +4391,9 @@
         <v>173</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11" t="n">
+        <v>76</v>
+      </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
     </row>
@@ -4397,7 +4409,9 @@
         <v>41</v>
       </c>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
@@ -4413,7 +4427,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="n">
         <f aca="false">SUM(F44:F48)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -4430,7 +4444,9 @@
         <v>174</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
@@ -4446,7 +4462,9 @@
         <v>44</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
@@ -4462,7 +4480,9 @@
         <v>45</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
@@ -4478,7 +4498,9 @@
         <v>46</v>
       </c>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
@@ -4494,7 +4516,9 @@
         <v>47</v>
       </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
@@ -4510,7 +4534,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10" t="n">
         <f aca="false">SUM(F50:F55)</f>
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4527,7 +4551,9 @@
         <v>49</v>
       </c>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="n">
+        <v>53</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
     </row>
@@ -4543,7 +4569,9 @@
         <v>163</v>
       </c>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="n">
+        <v>84</v>
+      </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
@@ -4559,7 +4587,9 @@
         <v>148</v>
       </c>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="n">
+        <v>56</v>
+      </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
     </row>
@@ -4575,7 +4605,9 @@
         <v>175</v>
       </c>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="F53" s="11" t="n">
+        <v>61</v>
+      </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
     </row>
@@ -4591,7 +4623,9 @@
         <v>191</v>
       </c>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="F54" s="11" t="n">
+        <v>85</v>
+      </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
@@ -4607,7 +4641,9 @@
         <v>192</v>
       </c>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11" t="n">
+        <v>380</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
     </row>
@@ -4623,7 +4659,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10" t="n">
         <f aca="false">SUM(F57:F65,F68)</f>
-        <v>0</v>
+        <v>607</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -4640,7 +4676,9 @@
         <v>56</v>
       </c>
       <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+      <c r="F57" s="11" t="n">
+        <v>59</v>
+      </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
     </row>
@@ -4656,7 +4694,9 @@
         <v>57</v>
       </c>
       <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="F58" s="11" t="n">
+        <v>61</v>
+      </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
     </row>
@@ -4672,7 +4712,9 @@
         <v>58</v>
       </c>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="F59" s="11" t="n">
+        <v>123</v>
+      </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
     </row>
@@ -4688,7 +4730,9 @@
         <v>142</v>
       </c>
       <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="F60" s="11" t="n">
+        <v>122</v>
+      </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
     </row>
@@ -4704,7 +4748,9 @@
         <v>60</v>
       </c>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="F61" s="11" t="n">
+        <v>26</v>
+      </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
     </row>
@@ -4720,7 +4766,9 @@
         <v>177</v>
       </c>
       <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="F62" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
     </row>
@@ -4736,7 +4784,9 @@
         <v>62</v>
       </c>
       <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="F63" s="11" t="n">
+        <v>57</v>
+      </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
     </row>
@@ -4752,7 +4802,9 @@
         <v>63</v>
       </c>
       <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
+      <c r="F64" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
     </row>
@@ -4770,7 +4822,7 @@
       <c r="E65" s="11"/>
       <c r="F65" s="18" t="n">
         <f aca="false">SUM(F66:F67)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -4785,7 +4837,9 @@
         <v>64</v>
       </c>
       <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
+      <c r="F66" s="16" t="n">
+        <v>1</v>
+      </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
     </row>
@@ -4799,7 +4853,9 @@
         <v>149</v>
       </c>
       <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="16" t="n">
+        <v>21</v>
+      </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
     </row>
@@ -4815,7 +4871,9 @@
         <v>178</v>
       </c>
       <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="F68" s="11" t="n">
+        <v>96</v>
+      </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
     </row>
@@ -4831,7 +4889,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="10" t="n">
         <f aca="false">SUM(F70:F73,F77)</f>
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
@@ -4848,7 +4906,9 @@
         <v>204</v>
       </c>
       <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="F70" s="11" t="n">
+        <v>72</v>
+      </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
     </row>
@@ -4864,7 +4924,9 @@
         <v>205</v>
       </c>
       <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="F71" s="11" t="n">
+        <v>145</v>
+      </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
     </row>
@@ -4880,7 +4942,9 @@
         <v>71</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+      <c r="F72" s="11" t="n">
+        <v>144</v>
+      </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
     </row>
@@ -4897,8 +4961,7 @@
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="11" t="n">
-        <f aca="false">SUM(F74:F76)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -4913,7 +4976,9 @@
         <v>73</v>
       </c>
       <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="16" t="n">
+        <v>40</v>
+      </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
     </row>
@@ -4927,7 +4992,9 @@
         <v>74</v>
       </c>
       <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
+      <c r="F75" s="16" t="n">
+        <v>123</v>
+      </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
     </row>
@@ -4941,7 +5008,9 @@
         <v>75</v>
       </c>
       <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
+      <c r="F76" s="16" t="n">
+        <v>5</v>
+      </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
@@ -4957,7 +5026,9 @@
         <v>76</v>
       </c>
       <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+      <c r="F77" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
     </row>
@@ -4973,7 +5044,7 @@
       <c r="E78" s="10"/>
       <c r="F78" s="10" t="n">
         <f aca="false">SUM(F79:F82,F86:F88,F92,F95,F98:F100,F103:F106)</f>
-        <v>0</v>
+        <v>1521</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
@@ -4990,7 +5061,9 @@
         <v>179</v>
       </c>
       <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="F79" s="11" t="n">
+        <v>84</v>
+      </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
     </row>
@@ -5006,7 +5079,9 @@
         <v>79</v>
       </c>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="F80" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
     </row>
@@ -5022,7 +5097,9 @@
         <v>80</v>
       </c>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
+      <c r="F81" s="11" t="n">
+        <v>71</v>
+      </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
     </row>
@@ -5040,7 +5117,7 @@
       <c r="E82" s="11"/>
       <c r="F82" s="11" t="n">
         <f aca="false">SUM(F83:F85)</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -5055,7 +5132,9 @@
         <v>150</v>
       </c>
       <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
+      <c r="F83" s="16" t="n">
+        <v>17</v>
+      </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
     </row>
@@ -5069,7 +5148,9 @@
         <v>151</v>
       </c>
       <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
+      <c r="F84" s="16" t="n">
+        <v>101</v>
+      </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
     </row>
@@ -5083,7 +5164,9 @@
         <v>152</v>
       </c>
       <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="F85" s="16" t="n">
+        <v>113</v>
+      </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
     </row>
@@ -5099,7 +5182,9 @@
         <v>82</v>
       </c>
       <c r="E86" s="11"/>
-      <c r="F86" s="17"/>
+      <c r="F86" s="17" t="n">
+        <v>3</v>
+      </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
     </row>
@@ -5115,7 +5200,9 @@
         <v>83</v>
       </c>
       <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="F87" s="11" t="n">
+        <v>28</v>
+      </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
     </row>
@@ -5133,7 +5220,7 @@
       <c r="E88" s="11"/>
       <c r="F88" s="11" t="n">
         <f aca="false">SUM(F89:F90)</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -5148,7 +5235,9 @@
         <v>84</v>
       </c>
       <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
+      <c r="F89" s="16" t="n">
+        <v>219</v>
+      </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
     </row>
@@ -5162,7 +5251,9 @@
         <v>153</v>
       </c>
       <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
+      <c r="F90" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
     </row>
@@ -5178,7 +5269,9 @@
         <v>85</v>
       </c>
       <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="F91" s="11" t="n">
+        <v>107</v>
+      </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
     </row>
@@ -5196,7 +5289,7 @@
       <c r="E92" s="11"/>
       <c r="F92" s="11" t="n">
         <f aca="false">SUM(F93:F94)</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -5211,7 +5304,9 @@
         <v>86</v>
       </c>
       <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
+      <c r="F93" s="16" t="n">
+        <v>86</v>
+      </c>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
     </row>
@@ -5225,7 +5320,9 @@
         <v>154</v>
       </c>
       <c r="E94" s="16"/>
-      <c r="F94" s="16"/>
+      <c r="F94" s="16" t="n">
+        <v>18</v>
+      </c>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
     </row>
@@ -5243,7 +5340,7 @@
       <c r="E95" s="11"/>
       <c r="F95" s="11" t="n">
         <f aca="false">SUM(F96:F97)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -5258,7 +5355,9 @@
         <v>87</v>
       </c>
       <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
+      <c r="F96" s="16" t="n">
+        <v>35</v>
+      </c>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
     </row>
@@ -5272,7 +5371,9 @@
         <v>155</v>
       </c>
       <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
+      <c r="F97" s="16" t="n">
+        <v>14</v>
+      </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
     </row>
@@ -5288,7 +5389,9 @@
         <v>88</v>
       </c>
       <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="F98" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
     </row>
@@ -5304,7 +5407,9 @@
         <v>89</v>
       </c>
       <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="F99" s="11" t="n">
+        <v>56</v>
+      </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
     </row>
@@ -5322,7 +5427,7 @@
       <c r="E100" s="11"/>
       <c r="F100" s="11" t="n">
         <f aca="false">SUM(F101:F102)</f>
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
@@ -5337,7 +5442,9 @@
         <v>65</v>
       </c>
       <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
+      <c r="F101" s="16" t="n">
+        <v>8</v>
+      </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
     </row>
@@ -5351,7 +5458,9 @@
         <v>156</v>
       </c>
       <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
+      <c r="F102" s="16" t="n">
+        <v>105</v>
+      </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
     </row>
@@ -5367,7 +5476,9 @@
         <v>92</v>
       </c>
       <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="F103" s="11" t="n">
+        <v>59</v>
+      </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
     </row>
@@ -5383,7 +5494,9 @@
         <v>93</v>
       </c>
       <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
+      <c r="F104" s="11" t="n">
+        <v>288</v>
+      </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
     </row>
@@ -5399,7 +5512,9 @@
         <v>94</v>
       </c>
       <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
+      <c r="F105" s="11" t="n">
+        <v>51</v>
+      </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
     </row>
@@ -5415,7 +5530,9 @@
         <v>95</v>
       </c>
       <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
+      <c r="F106" s="11" t="n">
+        <v>63</v>
+      </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
     </row>
@@ -5431,7 +5548,7 @@
       <c r="E107" s="10"/>
       <c r="F107" s="10" t="n">
         <f aca="false">SUM(F108:F111,F114:F123,F126,F129)</f>
-        <v>0</v>
+        <v>797</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
@@ -5448,7 +5565,9 @@
         <v>206</v>
       </c>
       <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
+      <c r="F108" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
     </row>
@@ -5464,7 +5583,9 @@
         <v>98</v>
       </c>
       <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
+      <c r="F109" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
     </row>
@@ -5480,7 +5601,9 @@
         <v>99</v>
       </c>
       <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
+      <c r="F110" s="11" t="n">
+        <v>46</v>
+      </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
@@ -5498,7 +5621,7 @@
       <c r="E111" s="11"/>
       <c r="F111" s="11" t="n">
         <f aca="false">SUM(F112:F113)</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
@@ -5513,7 +5636,9 @@
         <v>100</v>
       </c>
       <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
+      <c r="F112" s="11" t="n">
+        <v>71</v>
+      </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
     </row>
@@ -5527,7 +5652,9 @@
         <v>180</v>
       </c>
       <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="F113" s="11" t="n">
+        <v>63</v>
+      </c>
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
     </row>
@@ -5543,7 +5670,9 @@
         <v>144</v>
       </c>
       <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="F114" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
@@ -5559,7 +5688,9 @@
         <v>102</v>
       </c>
       <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
+      <c r="F115" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
@@ -5575,7 +5706,9 @@
         <v>185</v>
       </c>
       <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
+      <c r="F116" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
@@ -5591,7 +5724,9 @@
         <v>165</v>
       </c>
       <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
+      <c r="F117" s="11" t="n">
+        <v>41</v>
+      </c>
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
@@ -5607,7 +5742,9 @@
         <v>105</v>
       </c>
       <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+      <c r="F118" s="11" t="n">
+        <v>17</v>
+      </c>
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
@@ -5623,7 +5760,9 @@
         <v>207</v>
       </c>
       <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
+      <c r="F119" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
@@ -5639,7 +5778,9 @@
         <v>107</v>
       </c>
       <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
+      <c r="F120" s="11" t="n">
+        <v>102</v>
+      </c>
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
@@ -5655,7 +5796,9 @@
         <v>166</v>
       </c>
       <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
+      <c r="F121" s="11" t="n">
+        <v>172</v>
+      </c>
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
@@ -5671,7 +5814,9 @@
         <v>109</v>
       </c>
       <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
+      <c r="F122" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
@@ -5689,7 +5834,7 @@
       <c r="E123" s="11"/>
       <c r="F123" s="11" t="n">
         <f aca="false">SUM(F124:F125)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
@@ -5704,7 +5849,9 @@
         <v>65</v>
       </c>
       <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
+      <c r="F124" s="11" t="n">
+        <v>9</v>
+      </c>
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
@@ -5718,7 +5865,9 @@
         <v>111</v>
       </c>
       <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
+      <c r="F125" s="11" t="n">
+        <v>36</v>
+      </c>
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
@@ -5736,7 +5885,7 @@
       <c r="E126" s="11"/>
       <c r="F126" s="11" t="n">
         <f aca="false">SUM(F127:F128)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
@@ -5751,7 +5900,9 @@
         <v>65</v>
       </c>
       <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
+      <c r="F127" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
@@ -5765,7 +5916,9 @@
         <v>114</v>
       </c>
       <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
+      <c r="F128" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
@@ -5781,7 +5934,9 @@
         <v>115</v>
       </c>
       <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
+      <c r="F129" s="11" t="n">
+        <v>22</v>
+      </c>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
     </row>
@@ -5797,7 +5952,7 @@
       <c r="E130" s="10"/>
       <c r="F130" s="10" t="n">
         <f aca="false">SUM(F131:F135)</f>
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
@@ -5814,7 +5969,9 @@
         <v>196</v>
       </c>
       <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
+      <c r="F131" s="11" t="n">
+        <v>222</v>
+      </c>
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
     </row>
@@ -5830,7 +5987,9 @@
         <v>158</v>
       </c>
       <c r="E132" s="17"/>
-      <c r="F132" s="17"/>
+      <c r="F132" s="17" t="n">
+        <v>39</v>
+      </c>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
@@ -5846,7 +6005,9 @@
         <v>159</v>
       </c>
       <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
+      <c r="F133" s="17" t="n">
+        <v>18</v>
+      </c>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
@@ -5862,7 +6023,9 @@
         <v>118</v>
       </c>
       <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
+      <c r="F134" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
@@ -5878,7 +6041,9 @@
         <v>119</v>
       </c>
       <c r="E135" s="11"/>
-      <c r="F135" s="11"/>
+      <c r="F135" s="11" t="n">
+        <v>31</v>
+      </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
     </row>
@@ -5894,7 +6059,7 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10" t="n">
         <f aca="false">SUM(F137,F140,F143)</f>
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="G136" s="11"/>
       <c r="H136" s="11"/>
@@ -5913,7 +6078,7 @@
       <c r="E137" s="11"/>
       <c r="F137" s="11" t="n">
         <f aca="false">SUM(F138:F139)</f>
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="G137" s="11"/>
       <c r="H137" s="11"/>
@@ -5928,7 +6093,9 @@
         <v>123</v>
       </c>
       <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
+      <c r="F138" s="16" t="n">
+        <v>166</v>
+      </c>
       <c r="G138" s="11"/>
       <c r="H138" s="11"/>
     </row>
@@ -5942,7 +6109,9 @@
         <v>124</v>
       </c>
       <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
+      <c r="F139" s="16" t="n">
+        <v>52</v>
+      </c>
       <c r="G139" s="11"/>
       <c r="H139" s="11"/>
     </row>
@@ -5960,7 +6129,7 @@
       <c r="E140" s="11"/>
       <c r="F140" s="11" t="n">
         <f aca="false">SUM(F141:F142)</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
@@ -5975,7 +6144,9 @@
         <v>197</v>
       </c>
       <c r="E141" s="16"/>
-      <c r="F141" s="16"/>
+      <c r="F141" s="16" t="n">
+        <v>138</v>
+      </c>
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
     </row>
@@ -5989,7 +6160,9 @@
         <v>198</v>
       </c>
       <c r="E142" s="16"/>
-      <c r="F142" s="16"/>
+      <c r="F142" s="16" t="n">
+        <v>14</v>
+      </c>
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
     </row>
@@ -6005,7 +6178,9 @@
         <v>63</v>
       </c>
       <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
+      <c r="F143" s="11" t="n">
+        <v>78</v>
+      </c>
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
     </row>
@@ -6021,7 +6196,7 @@
       <c r="E144" s="10"/>
       <c r="F144" s="10" t="n">
         <f aca="false">SUM(F145:F152,F155:F158)</f>
-        <v>0</v>
+        <v>638</v>
       </c>
       <c r="G144" s="11"/>
       <c r="H144" s="11"/>
@@ -6038,7 +6213,9 @@
         <v>127</v>
       </c>
       <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
+      <c r="F145" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
     </row>
@@ -6054,7 +6231,9 @@
         <v>128</v>
       </c>
       <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
+      <c r="F146" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G146" s="11"/>
       <c r="H146" s="11"/>
     </row>
@@ -6070,7 +6249,9 @@
         <v>129</v>
       </c>
       <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
+      <c r="F147" s="11" t="n">
+        <v>35</v>
+      </c>
       <c r="G147" s="11"/>
       <c r="H147" s="11"/>
     </row>
@@ -6086,7 +6267,9 @@
         <v>130</v>
       </c>
       <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="F148" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="G148" s="11"/>
       <c r="H148" s="11"/>
     </row>
@@ -6102,7 +6285,9 @@
         <v>131</v>
       </c>
       <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
+      <c r="F149" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="G149" s="11"/>
       <c r="H149" s="11"/>
     </row>
@@ -6118,7 +6303,9 @@
         <v>199</v>
       </c>
       <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
+      <c r="F150" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G150" s="11"/>
       <c r="H150" s="11"/>
     </row>
@@ -6134,7 +6321,9 @@
         <v>200</v>
       </c>
       <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="F151" s="11" t="n">
+        <v>17</v>
+      </c>
       <c r="G151" s="11"/>
       <c r="H151" s="11"/>
     </row>
@@ -6152,7 +6341,7 @@
       <c r="E152" s="11"/>
       <c r="F152" s="11" t="n">
         <f aca="false">SUM(F153:F154)</f>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="G152" s="11"/>
       <c r="H152" s="11"/>
@@ -6167,7 +6356,9 @@
         <v>134</v>
       </c>
       <c r="E153" s="16"/>
-      <c r="F153" s="16"/>
+      <c r="F153" s="16" t="n">
+        <v>123</v>
+      </c>
       <c r="G153" s="11"/>
       <c r="H153" s="11"/>
     </row>
@@ -6181,7 +6372,9 @@
         <v>160</v>
       </c>
       <c r="E154" s="16"/>
-      <c r="F154" s="16"/>
+      <c r="F154" s="16" t="n">
+        <v>12</v>
+      </c>
       <c r="G154" s="11"/>
       <c r="H154" s="11"/>
     </row>
@@ -6197,7 +6390,9 @@
         <v>135</v>
       </c>
       <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
+      <c r="F155" s="11" t="n">
+        <v>14</v>
+      </c>
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
     </row>
@@ -6213,7 +6408,9 @@
         <v>136</v>
       </c>
       <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
+      <c r="F156" s="11" t="n">
+        <v>64</v>
+      </c>
       <c r="G156" s="11"/>
       <c r="H156" s="11"/>
     </row>
@@ -6229,7 +6426,9 @@
         <v>137</v>
       </c>
       <c r="E157" s="11"/>
-      <c r="F157" s="11"/>
+      <c r="F157" s="11" t="n">
+        <v>10</v>
+      </c>
       <c r="G157" s="11"/>
       <c r="H157" s="11"/>
     </row>
@@ -6245,7 +6444,9 @@
         <v>138</v>
       </c>
       <c r="E158" s="11"/>
-      <c r="F158" s="11"/>
+      <c r="F158" s="11" t="n">
+        <v>130</v>
+      </c>
       <c r="G158" s="11"/>
       <c r="H158" s="11"/>
     </row>
@@ -6311,7 +6512,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -6329,7 +6530,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="n">
         <f aca="false">SUM(F5:F19)</f>
-        <v>0</v>
+        <v>696</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -6362,7 +6563,9 @@
         <v>202</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="n">
+        <v>72</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
@@ -6378,7 +6581,9 @@
         <v>11</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="11" t="n">
+        <v>157</v>
+      </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
@@ -6394,7 +6599,9 @@
         <v>12</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="11" t="n">
+        <v>53</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
@@ -6410,7 +6617,9 @@
         <v>13</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
@@ -6458,7 +6667,9 @@
         <v>16</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="F12" s="11" t="n">
+        <v>138</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
@@ -6474,7 +6685,9 @@
         <v>17</v>
       </c>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
@@ -6490,7 +6703,9 @@
         <v>18</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
@@ -6506,7 +6721,9 @@
         <v>19</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="11" t="n">
+        <v>28</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
@@ -6522,7 +6739,9 @@
         <v>140</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
@@ -6538,7 +6757,9 @@
         <v>21</v>
       </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="11" t="n">
+        <v>33</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
@@ -6554,7 +6775,9 @@
         <v>22</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="11" t="n">
+        <v>48</v>
+      </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
@@ -6570,7 +6793,9 @@
         <v>23</v>
       </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
@@ -6586,7 +6811,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="n">
         <f aca="false">SUM(F21:F22)</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -6603,7 +6828,9 @@
         <v>168</v>
       </c>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="11" t="n">
+        <v>33</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
@@ -6619,7 +6846,9 @@
         <v>26</v>
       </c>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="11" t="n">
+        <v>124</v>
+      </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>
@@ -8807,8 +9036,8 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8851,7 +9080,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>853</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -8869,7 +9098,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="n">
         <f aca="false">SUM(F5:F19)</f>
-        <v>696</v>
+        <v>0</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -8902,9 +9131,7 @@
         <v>202</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="11" t="n">
-        <v>72</v>
-      </c>
+      <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
@@ -8920,9 +9147,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="11" t="n">
-        <v>157</v>
-      </c>
+      <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
@@ -8938,9 +9163,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="11" t="n">
-        <v>53</v>
-      </c>
+      <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
@@ -8956,9 +9179,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
@@ -9006,9 +9227,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="11" t="n">
-        <v>138</v>
-      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
@@ -9024,9 +9243,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="11"/>
-      <c r="F13" s="11" t="n">
-        <v>21</v>
-      </c>
+      <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
@@ -9042,9 +9259,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="11" t="n">
-        <v>47</v>
-      </c>
+      <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
@@ -9060,9 +9275,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="11" t="n">
-        <v>28</v>
-      </c>
+      <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
@@ -9078,9 +9291,7 @@
         <v>140</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="11" t="n">
-        <v>50</v>
-      </c>
+      <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
@@ -9096,9 +9307,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="11" t="n">
-        <v>33</v>
-      </c>
+      <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
@@ -9114,9 +9323,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11" t="n">
-        <v>48</v>
-      </c>
+      <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
@@ -9132,9 +9339,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="11" t="n">
-        <v>47</v>
-      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
@@ -9150,7 +9355,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="n">
         <f aca="false">SUM(F21:F22)</f>
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -9167,9 +9372,7 @@
         <v>168</v>
       </c>
       <c r="E21" s="11"/>
-      <c r="F21" s="11" t="n">
-        <v>33</v>
-      </c>
+      <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
@@ -9185,9 +9388,7 @@
         <v>26</v>
       </c>
       <c r="E22" s="11"/>
-      <c r="F22" s="11" t="n">
-        <v>124</v>
-      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>

</xml_diff>

<commit_message>
Added more entry counts
 On branch master

 Changes to be committed:
	modified:   Books20/Data/AAA/AAA_counts.xlsx
</commit_message>
<xml_diff>
--- a/Books20/Data/AAA/AAA_counts.xlsx
+++ b/Books20/Data/AAA/AAA_counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="AAA v9 1973.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -3681,7 +3681,7 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F159" activeCellId="0" sqref="F159"/>
     </sheetView>
   </sheetViews>
@@ -6468,8 +6468,8 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6512,7 +6512,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>853</v>
+        <v>2585</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -6864,7 +6864,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="n">
         <f aca="false">SUM(F24,F28, F31:F34)</f>
-        <v>0</v>
+        <v>485</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -6883,7 +6883,7 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11" t="n">
         <f aca="false">SUM(F25:F27)</f>
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -6898,7 +6898,9 @@
         <v>169</v>
       </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="F25" s="16" t="n">
+        <v>41</v>
+      </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
@@ -6912,7 +6914,9 @@
         <v>170</v>
       </c>
       <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="F26" s="16" t="n">
+        <v>119</v>
+      </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
     </row>
@@ -6926,7 +6930,9 @@
         <v>171</v>
       </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="16" t="n">
+        <v>24</v>
+      </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
@@ -6944,7 +6950,7 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11" t="n">
         <f aca="false">SUM(F29:F30)</f>
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -6959,7 +6965,9 @@
         <v>29</v>
       </c>
       <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="F29" s="16" t="n">
+        <v>74</v>
+      </c>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
@@ -6973,7 +6981,9 @@
         <v>184</v>
       </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
+      <c r="F30" s="16" t="n">
+        <v>79</v>
+      </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
     </row>
@@ -6989,7 +6999,9 @@
         <v>30</v>
       </c>
       <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="11" t="n">
+        <v>48</v>
+      </c>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
     </row>
@@ -7005,7 +7017,9 @@
         <v>31</v>
       </c>
       <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="F32" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
     </row>
@@ -7021,7 +7035,9 @@
         <v>32</v>
       </c>
       <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="F33" s="11" t="n">
+        <v>13</v>
+      </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
@@ -7037,7 +7053,9 @@
         <v>33</v>
       </c>
       <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="11" t="n">
+        <v>12</v>
+      </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
     </row>
@@ -7053,7 +7071,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="n">
         <f aca="false">SUM(F36:F42)</f>
-        <v>0</v>
+        <v>327</v>
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -7070,7 +7088,9 @@
         <v>203</v>
       </c>
       <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="n">
+        <v>43</v>
+      </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
@@ -7086,7 +7106,9 @@
         <v>172</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="11" t="n">
+        <v>143</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
@@ -7102,7 +7124,9 @@
         <v>37</v>
       </c>
       <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="11" t="n">
+        <v>12</v>
+      </c>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
@@ -7118,7 +7142,9 @@
         <v>38</v>
       </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11" t="n">
+        <v>38</v>
+      </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
@@ -7134,7 +7160,9 @@
         <v>39</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
@@ -7150,7 +7178,9 @@
         <v>173</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
     </row>
@@ -7166,7 +7196,9 @@
         <v>41</v>
       </c>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
@@ -7182,7 +7214,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10" t="n">
         <f aca="false">SUM(F44:F48)</f>
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -7199,7 +7231,9 @@
         <v>174</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="11" t="n">
+        <v>36</v>
+      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
@@ -7215,7 +7249,9 @@
         <v>44</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11" t="n">
+        <v>57</v>
+      </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
@@ -7231,7 +7267,9 @@
         <v>45</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="n">
+        <v>16</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
@@ -7247,7 +7285,9 @@
         <v>46</v>
       </c>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="n">
+        <v>27</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
@@ -7263,7 +7303,9 @@
         <v>47</v>
       </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="n">
+        <v>13</v>
+      </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
@@ -7279,7 +7321,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10" t="n">
         <f aca="false">SUM(F50:F55)</f>
-        <v>0</v>
+        <v>771</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -7296,7 +7338,9 @@
         <v>49</v>
       </c>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="n">
+        <v>58</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
     </row>
@@ -7312,7 +7356,9 @@
         <v>163</v>
       </c>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="n">
+        <v>119</v>
+      </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
@@ -7328,7 +7374,9 @@
         <v>148</v>
       </c>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
     </row>
@@ -7344,7 +7392,9 @@
         <v>175</v>
       </c>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="F53" s="11" t="n">
+        <v>113</v>
+      </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
     </row>
@@ -7360,7 +7410,9 @@
         <v>191</v>
       </c>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="F54" s="11" t="n">
+        <v>90</v>
+      </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
@@ -7376,7 +7428,9 @@
         <v>192</v>
       </c>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11" t="n">
+        <v>346</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
     </row>

</xml_diff>

<commit_message>
Finished entry counts for AAA 21
Updated ajb.ods

 On branch master

 Changes to be committed:
	modified:   Books20/Data/AAA/AAA_counts.xlsx
	modified:   Books20/Data/Ajb/ajb.ods
</commit_message>
<xml_diff>
--- a/Books20/Data/AAA/AAA_counts.xlsx
+++ b/Books20/Data/AAA/AAA_counts.xlsx
@@ -6468,8 +6468,8 @@
   </sheetPr>
   <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6512,7 +6512,7 @@
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">SUM(F4,F20,F23,F35,F43,F49,F56,F69,F78,F107,F130,F136,F144)</f>
-        <v>2585</v>
+        <v>8080</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>7</v>
@@ -7446,7 +7446,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10" t="n">
         <f aca="false">SUM(F57:F65,F68)</f>
-        <v>0</v>
+        <v>556</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -7463,7 +7463,9 @@
         <v>56</v>
       </c>
       <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+      <c r="F57" s="11" t="n">
+        <v>54</v>
+      </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
     </row>
@@ -7479,7 +7481,9 @@
         <v>57</v>
       </c>
       <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="F58" s="11" t="n">
+        <v>66</v>
+      </c>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
     </row>
@@ -7495,7 +7499,9 @@
         <v>58</v>
       </c>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="F59" s="11" t="n">
+        <v>101</v>
+      </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
     </row>
@@ -7511,7 +7517,9 @@
         <v>142</v>
       </c>
       <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="F60" s="11" t="n">
+        <v>100</v>
+      </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
     </row>
@@ -7527,7 +7535,9 @@
         <v>60</v>
       </c>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="F61" s="11" t="n">
+        <v>21</v>
+      </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
     </row>
@@ -7543,7 +7553,9 @@
         <v>177</v>
       </c>
       <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="F62" s="11" t="n">
+        <v>48</v>
+      </c>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
     </row>
@@ -7559,7 +7571,9 @@
         <v>62</v>
       </c>
       <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="F63" s="11" t="n">
+        <v>57</v>
+      </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
     </row>
@@ -7575,7 +7589,9 @@
         <v>63</v>
       </c>
       <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
+      <c r="F64" s="11" t="n">
+        <v>19</v>
+      </c>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
     </row>
@@ -7593,7 +7609,7 @@
       <c r="E65" s="11"/>
       <c r="F65" s="18" t="n">
         <f aca="false">SUM(F66:F67)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -7608,7 +7624,9 @@
         <v>64</v>
       </c>
       <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
+      <c r="F66" s="16" t="n">
+        <v>0</v>
+      </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
     </row>
@@ -7622,7 +7640,9 @@
         <v>149</v>
       </c>
       <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="16" t="n">
+        <v>16</v>
+      </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
     </row>
@@ -7638,7 +7658,9 @@
         <v>178</v>
       </c>
       <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="F68" s="11" t="n">
+        <v>74</v>
+      </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
     </row>
@@ -7654,7 +7676,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="10" t="n">
         <f aca="false">SUM(F70:F73,F77)</f>
-        <v>0</v>
+        <v>557</v>
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
@@ -7671,7 +7693,9 @@
         <v>204</v>
       </c>
       <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="F70" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
     </row>
@@ -7687,7 +7711,9 @@
         <v>205</v>
       </c>
       <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="F71" s="11" t="n">
+        <v>132</v>
+      </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
     </row>
@@ -7703,7 +7729,9 @@
         <v>71</v>
       </c>
       <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+      <c r="F72" s="11" t="n">
+        <v>141</v>
+      </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
     </row>
@@ -7721,7 +7749,7 @@
       <c r="E73" s="11"/>
       <c r="F73" s="11" t="n">
         <f aca="false">SUM(F74:F76)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -7736,7 +7764,9 @@
         <v>73</v>
       </c>
       <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="16" t="n">
+        <v>34</v>
+      </c>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
     </row>
@@ -7750,7 +7780,9 @@
         <v>209</v>
       </c>
       <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
+      <c r="F75" s="16" t="n">
+        <v>132</v>
+      </c>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
     </row>
@@ -7764,7 +7796,9 @@
         <v>75</v>
       </c>
       <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
+      <c r="F76" s="16" t="n">
+        <v>10</v>
+      </c>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
@@ -7780,7 +7814,9 @@
         <v>76</v>
       </c>
       <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+      <c r="F77" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
     </row>
@@ -7796,7 +7832,7 @@
       <c r="E78" s="10"/>
       <c r="F78" s="10" t="n">
         <f aca="false">SUM(F79:F82,F86:F88,F92,F95,F98:F100,F103:F106)</f>
-        <v>0</v>
+        <v>1178</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
@@ -7813,7 +7849,9 @@
         <v>179</v>
       </c>
       <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="F79" s="11" t="n">
+        <v>91</v>
+      </c>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
     </row>
@@ -7829,7 +7867,9 @@
         <v>79</v>
       </c>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="F80" s="11" t="n">
+        <v>23</v>
+      </c>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
     </row>
@@ -7845,7 +7885,9 @@
         <v>80</v>
       </c>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
+      <c r="F81" s="11" t="n">
+        <v>57</v>
+      </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
     </row>
@@ -7863,7 +7905,7 @@
       <c r="E82" s="11"/>
       <c r="F82" s="11" t="n">
         <f aca="false">SUM(F83:F85)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
@@ -7878,7 +7920,9 @@
         <v>150</v>
       </c>
       <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
+      <c r="F83" s="16" t="n">
+        <v>23</v>
+      </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
     </row>
@@ -7892,7 +7936,9 @@
         <v>151</v>
       </c>
       <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
+      <c r="F84" s="16" t="n">
+        <v>60</v>
+      </c>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
     </row>
@@ -7906,7 +7952,9 @@
         <v>152</v>
       </c>
       <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="F85" s="16" t="n">
+        <v>76</v>
+      </c>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
     </row>
@@ -7922,7 +7970,9 @@
         <v>82</v>
       </c>
       <c r="E86" s="11"/>
-      <c r="F86" s="17"/>
+      <c r="F86" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
     </row>
@@ -7938,7 +7988,9 @@
         <v>83</v>
       </c>
       <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="F87" s="11" t="n">
+        <v>14</v>
+      </c>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
     </row>
@@ -7956,7 +8008,7 @@
       <c r="E88" s="11"/>
       <c r="F88" s="11" t="n">
         <f aca="false">SUM(F89:F90)</f>
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -7971,7 +8023,9 @@
         <v>84</v>
       </c>
       <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
+      <c r="F89" s="16" t="n">
+        <v>177</v>
+      </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
     </row>
@@ -7985,7 +8039,9 @@
         <v>153</v>
       </c>
       <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
+      <c r="F90" s="16" t="n">
+        <v>27</v>
+      </c>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
     </row>
@@ -8001,7 +8057,9 @@
         <v>85</v>
       </c>
       <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="F91" s="11" t="n">
+        <v>100</v>
+      </c>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
     </row>
@@ -8019,7 +8077,7 @@
       <c r="E92" s="11"/>
       <c r="F92" s="11" t="n">
         <f aca="false">SUM(F93:F94)</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -8034,7 +8092,9 @@
         <v>86</v>
       </c>
       <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
+      <c r="F93" s="16" t="n">
+        <v>59</v>
+      </c>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
     </row>
@@ -8048,7 +8108,9 @@
         <v>154</v>
       </c>
       <c r="E94" s="16"/>
-      <c r="F94" s="16"/>
+      <c r="F94" s="16" t="n">
+        <v>40</v>
+      </c>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
     </row>
@@ -8066,7 +8128,7 @@
       <c r="E95" s="11"/>
       <c r="F95" s="11" t="n">
         <f aca="false">SUM(F96:F97)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -8081,7 +8143,9 @@
         <v>87</v>
       </c>
       <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
+      <c r="F96" s="16" t="n">
+        <v>43</v>
+      </c>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
     </row>
@@ -8095,7 +8159,9 @@
         <v>155</v>
       </c>
       <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
+      <c r="F97" s="16" t="n">
+        <v>9</v>
+      </c>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
     </row>
@@ -8111,7 +8177,9 @@
         <v>88</v>
       </c>
       <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="F98" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
     </row>
@@ -8127,7 +8195,9 @@
         <v>89</v>
       </c>
       <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="F99" s="11" t="n">
+        <v>41</v>
+      </c>
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
     </row>
@@ -8145,7 +8215,7 @@
       <c r="E100" s="11"/>
       <c r="F100" s="11" t="n">
         <f aca="false">SUM(F101:F102)</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
@@ -8160,7 +8230,9 @@
         <v>65</v>
       </c>
       <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
+      <c r="F101" s="16" t="n">
+        <v>14</v>
+      </c>
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
     </row>
@@ -8174,7 +8246,9 @@
         <v>156</v>
       </c>
       <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
+      <c r="F102" s="16" t="n">
+        <v>90</v>
+      </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
     </row>
@@ -8190,7 +8264,9 @@
         <v>92</v>
       </c>
       <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="F103" s="11" t="n">
+        <v>49</v>
+      </c>
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
     </row>
@@ -8206,7 +8282,9 @@
         <v>93</v>
       </c>
       <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
+      <c r="F104" s="11" t="n">
+        <v>118</v>
+      </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
     </row>
@@ -8222,7 +8300,9 @@
         <v>94</v>
       </c>
       <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
+      <c r="F105" s="11" t="n">
+        <v>69</v>
+      </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
     </row>
@@ -8238,7 +8318,9 @@
         <v>95</v>
       </c>
       <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
+      <c r="F106" s="11" t="n">
+        <v>49</v>
+      </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
     </row>
@@ -8254,7 +8336,7 @@
       <c r="E107" s="10"/>
       <c r="F107" s="10" t="n">
         <f aca="false">SUM(F108:F111,F114:F123,F126,F129)</f>
-        <v>0</v>
+        <v>1080</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
@@ -8271,7 +8353,9 @@
         <v>206</v>
       </c>
       <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
+      <c r="F108" s="11" t="n">
+        <v>9</v>
+      </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
     </row>
@@ -8287,7 +8371,9 @@
         <v>98</v>
       </c>
       <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
+      <c r="F109" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
     </row>
@@ -8303,7 +8389,9 @@
         <v>99</v>
       </c>
       <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
+      <c r="F110" s="11" t="n">
+        <v>93</v>
+      </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
@@ -8321,7 +8409,7 @@
       <c r="E111" s="11"/>
       <c r="F111" s="11" t="n">
         <f aca="false">SUM(F112:F113)</f>
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
@@ -8336,7 +8424,9 @@
         <v>100</v>
       </c>
       <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
+      <c r="F112" s="11" t="n">
+        <v>99</v>
+      </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
     </row>
@@ -8350,7 +8440,9 @@
         <v>180</v>
       </c>
       <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="F113" s="11" t="n">
+        <v>83</v>
+      </c>
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
     </row>
@@ -8366,7 +8458,9 @@
         <v>144</v>
       </c>
       <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="F114" s="11" t="n">
+        <v>19</v>
+      </c>
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
@@ -8382,7 +8476,9 @@
         <v>210</v>
       </c>
       <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
+      <c r="F115" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
@@ -8398,7 +8494,9 @@
         <v>185</v>
       </c>
       <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
+      <c r="F116" s="11" t="n">
+        <v>85</v>
+      </c>
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
@@ -8414,7 +8512,9 @@
         <v>165</v>
       </c>
       <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
+      <c r="F117" s="11" t="n">
+        <v>41</v>
+      </c>
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
@@ -8430,7 +8530,9 @@
         <v>105</v>
       </c>
       <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+      <c r="F118" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
@@ -8446,7 +8548,9 @@
         <v>207</v>
       </c>
       <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
+      <c r="F119" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
@@ -8462,7 +8566,9 @@
         <v>107</v>
       </c>
       <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
+      <c r="F120" s="11" t="n">
+        <v>103</v>
+      </c>
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
@@ -8478,7 +8584,9 @@
         <v>166</v>
       </c>
       <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
+      <c r="F121" s="11" t="n">
+        <v>214</v>
+      </c>
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
@@ -8494,7 +8602,9 @@
         <v>109</v>
       </c>
       <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
+      <c r="F122" s="11" t="n">
+        <v>74</v>
+      </c>
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
@@ -8512,7 +8622,7 @@
       <c r="E123" s="11"/>
       <c r="F123" s="11" t="n">
         <f aca="false">SUM(F124:F125)</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
@@ -8527,7 +8637,9 @@
         <v>65</v>
       </c>
       <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
+      <c r="F124" s="11" t="n">
+        <v>28</v>
+      </c>
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
@@ -8541,7 +8653,9 @@
         <v>111</v>
       </c>
       <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
+      <c r="F125" s="11" t="n">
+        <v>46</v>
+      </c>
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
@@ -8559,7 +8673,7 @@
       <c r="E126" s="11"/>
       <c r="F126" s="11" t="n">
         <f aca="false">SUM(F127:F128)</f>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
@@ -8574,7 +8688,9 @@
         <v>65</v>
       </c>
       <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
+      <c r="F127" s="11" t="n">
+        <v>77</v>
+      </c>
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
@@ -8588,7 +8704,9 @@
         <v>114</v>
       </c>
       <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
+      <c r="F128" s="11" t="n">
+        <v>0</v>
+      </c>
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
@@ -8604,7 +8722,9 @@
         <v>211</v>
       </c>
       <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
+      <c r="F129" s="11" t="n">
+        <v>42</v>
+      </c>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
     </row>
@@ -8620,7 +8740,7 @@
       <c r="E130" s="10"/>
       <c r="F130" s="10" t="n">
         <f aca="false">SUM(F131:F135)</f>
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
@@ -8637,7 +8757,9 @@
         <v>196</v>
       </c>
       <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
+      <c r="F131" s="11" t="n">
+        <v>261</v>
+      </c>
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
     </row>
@@ -8653,7 +8775,9 @@
         <v>158</v>
       </c>
       <c r="E132" s="17"/>
-      <c r="F132" s="17"/>
+      <c r="F132" s="17" t="n">
+        <v>73</v>
+      </c>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
@@ -8669,7 +8793,9 @@
         <v>159</v>
       </c>
       <c r="E133" s="17"/>
-      <c r="F133" s="17"/>
+      <c r="F133" s="17" t="n">
+        <v>50</v>
+      </c>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
@@ -8685,7 +8811,9 @@
         <v>118</v>
       </c>
       <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
+      <c r="F134" s="11" t="n">
+        <v>47</v>
+      </c>
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
@@ -8701,7 +8829,9 @@
         <v>119</v>
       </c>
       <c r="E135" s="11"/>
-      <c r="F135" s="11"/>
+      <c r="F135" s="11" t="n">
+        <v>109</v>
+      </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
     </row>
@@ -8717,7 +8847,7 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10" t="n">
         <f aca="false">SUM(F137,F140,F143)</f>
-        <v>0</v>
+        <v>641</v>
       </c>
       <c r="G136" s="11"/>
       <c r="H136" s="11"/>
@@ -8736,7 +8866,7 @@
       <c r="E137" s="11"/>
       <c r="F137" s="11" t="n">
         <f aca="false">SUM(F138:F139)</f>
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="G137" s="11"/>
       <c r="H137" s="11"/>
@@ -8751,7 +8881,9 @@
         <v>123</v>
       </c>
       <c r="E138" s="16"/>
-      <c r="F138" s="16"/>
+      <c r="F138" s="16" t="n">
+        <v>233</v>
+      </c>
       <c r="G138" s="11"/>
       <c r="H138" s="11"/>
     </row>
@@ -8765,7 +8897,9 @@
         <v>124</v>
       </c>
       <c r="E139" s="16"/>
-      <c r="F139" s="16"/>
+      <c r="F139" s="16" t="n">
+        <v>56</v>
+      </c>
       <c r="G139" s="11"/>
       <c r="H139" s="11"/>
     </row>
@@ -8783,7 +8917,7 @@
       <c r="E140" s="11"/>
       <c r="F140" s="11" t="n">
         <f aca="false">SUM(F141:F142)</f>
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
@@ -8798,7 +8932,9 @@
         <v>197</v>
       </c>
       <c r="E141" s="16"/>
-      <c r="F141" s="16"/>
+      <c r="F141" s="16" t="n">
+        <v>247</v>
+      </c>
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
     </row>
@@ -8812,7 +8948,9 @@
         <v>198</v>
       </c>
       <c r="E142" s="16"/>
-      <c r="F142" s="16"/>
+      <c r="F142" s="16" t="n">
+        <v>33</v>
+      </c>
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
     </row>
@@ -8828,7 +8966,9 @@
         <v>63</v>
       </c>
       <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
+      <c r="F143" s="11" t="n">
+        <v>72</v>
+      </c>
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
     </row>
@@ -8844,7 +8984,7 @@
       <c r="E144" s="10"/>
       <c r="F144" s="10" t="n">
         <f aca="false">SUM(F145:F152,F155:F158)</f>
-        <v>0</v>
+        <v>943</v>
       </c>
       <c r="G144" s="11"/>
       <c r="H144" s="11"/>
@@ -8861,7 +9001,9 @@
         <v>127</v>
       </c>
       <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
+      <c r="F145" s="11" t="n">
+        <v>127</v>
+      </c>
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
     </row>
@@ -8877,7 +9019,9 @@
         <v>128</v>
       </c>
       <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
+      <c r="F146" s="11" t="n">
+        <v>6</v>
+      </c>
       <c r="G146" s="11"/>
       <c r="H146" s="11"/>
     </row>
@@ -8893,7 +9037,9 @@
         <v>129</v>
       </c>
       <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
+      <c r="F147" s="11" t="n">
+        <v>48</v>
+      </c>
       <c r="G147" s="11"/>
       <c r="H147" s="11"/>
     </row>
@@ -8909,7 +9055,9 @@
         <v>130</v>
       </c>
       <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="F148" s="11" t="n">
+        <v>42</v>
+      </c>
       <c r="G148" s="11"/>
       <c r="H148" s="11"/>
     </row>
@@ -8925,7 +9073,9 @@
         <v>131</v>
       </c>
       <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
+      <c r="F149" s="11" t="n">
+        <v>66</v>
+      </c>
       <c r="G149" s="11"/>
       <c r="H149" s="11"/>
     </row>
@@ -8941,7 +9091,9 @@
         <v>199</v>
       </c>
       <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
+      <c r="F150" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="G150" s="11"/>
       <c r="H150" s="11"/>
     </row>
@@ -8957,7 +9109,9 @@
         <v>200</v>
       </c>
       <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="F151" s="11" t="n">
+        <v>11</v>
+      </c>
       <c r="G151" s="11"/>
       <c r="H151" s="11"/>
     </row>
@@ -8975,7 +9129,7 @@
       <c r="E152" s="11"/>
       <c r="F152" s="11" t="n">
         <f aca="false">SUM(F153:F154)</f>
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="G152" s="11"/>
       <c r="H152" s="11"/>
@@ -8990,7 +9144,9 @@
         <v>134</v>
       </c>
       <c r="E153" s="16"/>
-      <c r="F153" s="16"/>
+      <c r="F153" s="16" t="n">
+        <v>279</v>
+      </c>
       <c r="G153" s="11"/>
       <c r="H153" s="11"/>
     </row>
@@ -9004,7 +9160,9 @@
         <v>160</v>
       </c>
       <c r="E154" s="16"/>
-      <c r="F154" s="16"/>
+      <c r="F154" s="16" t="n">
+        <v>18</v>
+      </c>
       <c r="G154" s="11"/>
       <c r="H154" s="11"/>
     </row>
@@ -9020,7 +9178,9 @@
         <v>135</v>
       </c>
       <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
+      <c r="F155" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
     </row>
@@ -9036,7 +9196,9 @@
         <v>136</v>
       </c>
       <c r="E156" s="11"/>
-      <c r="F156" s="11"/>
+      <c r="F156" s="11" t="n">
+        <v>101</v>
+      </c>
       <c r="G156" s="11"/>
       <c r="H156" s="11"/>
     </row>
@@ -9052,7 +9214,9 @@
         <v>137</v>
       </c>
       <c r="E157" s="11"/>
-      <c r="F157" s="11"/>
+      <c r="F157" s="11" t="n">
+        <v>11</v>
+      </c>
       <c r="G157" s="11"/>
       <c r="H157" s="11"/>
     </row>
@@ -9068,7 +9232,9 @@
         <v>138</v>
       </c>
       <c r="E158" s="11"/>
-      <c r="F158" s="11"/>
+      <c r="F158" s="11" t="n">
+        <v>189</v>
+      </c>
       <c r="G158" s="11"/>
       <c r="H158" s="11"/>
     </row>

</xml_diff>